<commit_message>
adjust subplot and fix excel writing
</commit_message>
<xml_diff>
--- a/data/clean/jun_21_dec_24_error_check.xlsx
+++ b/data/clean/jun_21_dec_24_error_check.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Midnight samples" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Time mismatch" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Midnight samples" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,6 +430,3166 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:R48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>serial_num</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>sample_time</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pond_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>time_of_day</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pond_status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>equipment</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>do_mg_per_L</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>turbidity_cm</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>tds_ppt</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ammonia_mg_per_L</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>follow_up</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>month_year</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>hour</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>time_mismatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>3293</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5023</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>04:17</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>WG-SRV1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ara v12 monthly</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Taiwan #1</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>11</v>
+      </c>
+      <c r="K2" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2023-09</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>4</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>3294</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5022</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>04:08</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>WG-GOW1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ara v12 monthly</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Taiwan #1</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2023-09</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3295</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5021</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>04:01</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>WG-GOW2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ara v12 monthly</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Taiwan #1</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2023-09</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>5004</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2610</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>44851</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>07:17</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WG-VRM1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="L5" t="n">
+        <v>38</v>
+      </c>
+      <c r="M5" t="n">
+        <v>781</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2022-10</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>7</v>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5019</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2595</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44847</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>17:42</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>WG-NRO1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>8.140000000000001</v>
+      </c>
+      <c r="L6" t="n">
+        <v>24</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2022-10</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>17</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5351</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2263</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>WG-BSE1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>YSI Pro Quattro</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K7" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>22</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3.792</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2022-08</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>14</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>5504</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2110</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>44771</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10:08</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>WG-KSS1</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Assessment</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>YSI Pro Quattro</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="L8" t="n">
+        <v>30</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3.505</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2022-07</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>10</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>5774</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1840</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>44726</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11:57</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>WG-GRA1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>YSI Pro Quattro</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>8.640000000000001</v>
+      </c>
+      <c r="L9" t="n">
+        <v>28</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.515</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2022-06</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>11</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>5839</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1774</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>44716</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NL-NAR1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Assessment</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>7.37</v>
+      </c>
+      <c r="L10" t="n">
+        <v>34</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2022-06</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>17</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>5941</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1673</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>44704</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>04:30</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>NL-FAY1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="L11" t="n">
+        <v>34</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2022-05</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>6055</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1558</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>44687</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>10:38</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NL-PSR2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8.369999999999999</v>
+      </c>
+      <c r="L12" t="n">
+        <v>26</v>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2022-05</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>10</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>6182</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1431</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>44670</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>04:40</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>WG-AJU1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="L13" t="n">
+        <v>22</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>4</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>6192</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1421</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>44669</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>16:16</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>WG-KRO1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="L14" t="n">
+        <v>20</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>16</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>6202</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1411</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>44669</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>04:50</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>WG-KRO1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="K15" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="L15" t="n">
+        <v>25</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>4</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>6226</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1387</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>44664</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>15:52</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>WG-MUR1</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>8.31</v>
+      </c>
+      <c r="L16" t="n">
+        <v>19</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>15</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>6235</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1378</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>44664</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>05:30</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>WG-MUR2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K17" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="L17" t="n">
+        <v>20</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="b">
+        <v>0</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>5</v>
+      </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>6377</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>44644</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>05:10</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>NL-BAS1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="K18" t="n">
+        <v>8.06</v>
+      </c>
+      <c r="L18" t="n">
+        <v>25</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2022-03</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>5</v>
+      </c>
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>6492</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1122</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>WG-UCU1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>YSI Pro Quattro</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="L19" t="n">
+        <v>15</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.009</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="O19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2022-03</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>17</v>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>6499</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1114</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>07:36</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>WG-UCU1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>YSI Pro Quattro</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="K20" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L20" t="n">
+        <v>16</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="b">
+        <v>0</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>2022-03</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>7</v>
+      </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>7197</v>
+      </c>
+      <c r="B21" t="n">
+        <v>414</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>07:26</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>WG-SKD1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>8</v>
+      </c>
+      <c r="L21" t="n">
+        <v>19</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1.321</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>7</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>7225</v>
+      </c>
+      <c r="B22" t="n">
+        <v>386</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>10:04</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>WG-VRM2</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="K22" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="L22" t="n">
+        <v>17</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1.271</v>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>10</v>
+      </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>7227</v>
+      </c>
+      <c r="B23" t="n">
+        <v>384</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>07:26</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>WG-SPD2</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>7</v>
+      </c>
+      <c r="K23" t="n">
+        <v>7.99</v>
+      </c>
+      <c r="L23" t="n">
+        <v>9</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>7</v>
+      </c>
+      <c r="R23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>7231</v>
+      </c>
+      <c r="B24" t="n">
+        <v>380</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>11:16</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>WG-SVV1</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="K24" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="L24" t="n">
+        <v>22</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>11</v>
+      </c>
+      <c r="R24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>7237</v>
+      </c>
+      <c r="B25" t="n">
+        <v>374</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>44508</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>18:26</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>WG-VRM1</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="K25" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="L25" t="n">
+        <v>31</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.712</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>18</v>
+      </c>
+      <c r="R25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>7238</v>
+      </c>
+      <c r="B26" t="n">
+        <v>373</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>44508</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>WG-CBU1</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>8.130000000000001</v>
+      </c>
+      <c r="L26" t="n">
+        <v>19</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>9</v>
+      </c>
+      <c r="R26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>7240</v>
+      </c>
+      <c r="B27" t="n">
+        <v>371</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>44508</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>03:21</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>WG-VRM1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="K27" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="L27" t="n">
+        <v>33</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>2021-11</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>3</v>
+      </c>
+      <c r="R27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>7259</v>
+      </c>
+      <c r="B28" t="n">
+        <v>352</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>05:02</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>WG-SKD2</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="K28" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="n">
+        <v>0.341</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>5</v>
+      </c>
+      <c r="R28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>7260</v>
+      </c>
+      <c r="B29" t="n">
+        <v>351</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>03:36</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>WG-SKD1</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="K29" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>3</v>
+      </c>
+      <c r="R29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>7279</v>
+      </c>
+      <c r="B30" t="n">
+        <v>331</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>NL-MUN1</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="K30" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>7280</v>
+      </c>
+      <c r="B31" t="n">
+        <v>332</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>NL-SKB1</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K31" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>7286</v>
+      </c>
+      <c r="B32" t="n">
+        <v>325</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>18:19</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>WG-SVV1</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="n">
+        <v>3</v>
+      </c>
+      <c r="K32" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>18</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>7319</v>
+      </c>
+      <c r="B33" t="n">
+        <v>292</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>18:18</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>WG-SRO2</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K33" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O33" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>18</v>
+      </c>
+      <c r="R33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>7329</v>
+      </c>
+      <c r="B34" t="n">
+        <v>282</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>04:47</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>WG-SRO2</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>7.92</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O34" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>4</v>
+      </c>
+      <c r="R34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>7330</v>
+      </c>
+      <c r="B35" t="n">
+        <v>281</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>04:42</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>WG-SRO1</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="K35" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O35" t="b">
+        <v>0</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>2021-10</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>4</v>
+      </c>
+      <c r="R35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>7366</v>
+      </c>
+      <c r="B36" t="n">
+        <v>245</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>44467</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>05:11</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>NL-VJY1</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="K36" t="n">
+        <v>8.529999999999999</v>
+      </c>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="b">
+        <v>0</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q36" t="n">
+        <v>5</v>
+      </c>
+      <c r="R36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>7368</v>
+      </c>
+      <c r="B37" t="n">
+        <v>243</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>05:42</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>NL-MAS1</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="K37" t="n">
+        <v>8.35</v>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="b">
+        <v>0</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q37" t="n">
+        <v>5</v>
+      </c>
+      <c r="R37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>7374</v>
+      </c>
+      <c r="B38" t="n">
+        <v>237</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>44463</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>06:25</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>NL-MUN1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="K38" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q38" t="n">
+        <v>6</v>
+      </c>
+      <c r="R38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>7376</v>
+      </c>
+      <c r="B39" t="n">
+        <v>235</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>44463</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>05:48</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>NL-MAN1</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="K39" t="n">
+        <v>8.609999999999999</v>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q39" t="n">
+        <v>5</v>
+      </c>
+      <c r="R39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>7377</v>
+      </c>
+      <c r="B40" t="n">
+        <v>234</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>18:20</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>WG-SRO1</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="K40" t="n">
+        <v>7.42</v>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>18</v>
+      </c>
+      <c r="R40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>7382</v>
+      </c>
+      <c r="B41" t="n">
+        <v>229</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>WG-SRO2</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K41" t="n">
+        <v>7.59</v>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O41" t="b">
+        <v>0</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q41" t="n">
+        <v>5</v>
+      </c>
+      <c r="R41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>7418</v>
+      </c>
+      <c r="B42" t="n">
+        <v>193</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>06:25</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>WG-SPD2</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="K42" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O42" t="b">
+        <v>0</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q42" t="n">
+        <v>6</v>
+      </c>
+      <c r="R42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>7429</v>
+      </c>
+      <c r="B43" t="n">
+        <v>182</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>NL-VEN1</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="K43" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="b">
+        <v>0</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q43" t="n">
+        <v>5</v>
+      </c>
+      <c r="R43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>7430</v>
+      </c>
+      <c r="B44" t="n">
+        <v>181</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>04:40</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>NL-VJY1</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="K44" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="b">
+        <v>0</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q44" t="n">
+        <v>4</v>
+      </c>
+      <c r="R44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>7439</v>
+      </c>
+      <c r="B45" t="n">
+        <v>172</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>NL-SRI1</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="K45" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="b">
+        <v>0</v>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q45" t="n">
+        <v>5</v>
+      </c>
+      <c r="R45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>7440</v>
+      </c>
+      <c r="B46" t="n">
+        <v>171</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>44447</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>05:10</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>NL-MUN1</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="K46" t="n">
+        <v>8.51</v>
+      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="b">
+        <v>0</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>2021-09</t>
+        </is>
+      </c>
+      <c r="Q46" t="n">
+        <v>5</v>
+      </c>
+      <c r="R46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>7602</v>
+      </c>
+      <c r="B47" t="n">
+        <v>7</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>44383</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>NL-MUN1</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="b">
+        <v>0</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>2021-07</t>
+        </is>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>7607</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>44366</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>NL-SKB1</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Evening</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Ara v1 2 weekly</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="K48" t="n">
+        <v>8.140000000000001</v>
+      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="b">
+        <v>0</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>2021-06</t>
+        </is>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
push latest dataset clean
</commit_message>
<xml_diff>
--- a/data/clean/jun_21_dec_24_error_check.xlsx
+++ b/data/clean/jun_21_dec_24_error_check.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>serial_num</t>
+          <t>sample_idx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -496,30 +496,25 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>tds_ppt</t>
+          <t>ammonia_mg_per_L</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>ammonia_mg_per_L</t>
+          <t>follow_up</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>follow_up</t>
+          <t>month_year</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>month_year</t>
+          <t>hour</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>hour</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>time_mismatch</t>
         </is>
@@ -573,19 +568,18 @@
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="inlineStr">
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2023-09</t>
         </is>
       </c>
-      <c r="Q2" t="n">
+      <c r="P2" t="n">
         <v>4</v>
       </c>
-      <c r="R2" t="b">
+      <c r="Q2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -637,19 +631,18 @@
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" t="inlineStr">
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2023-09</t>
         </is>
       </c>
-      <c r="Q3" t="n">
+      <c r="P3" t="n">
         <v>4</v>
       </c>
-      <c r="R3" t="b">
+      <c r="Q3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -701,19 +694,18 @@
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" t="inlineStr">
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2023-09</t>
         </is>
       </c>
-      <c r="Q4" t="n">
+      <c r="P4" t="n">
         <v>4</v>
       </c>
-      <c r="R4" t="b">
+      <c r="Q4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -767,23 +759,20 @@
         <v>38</v>
       </c>
       <c r="M5" t="n">
-        <v>781</v>
-      </c>
-      <c r="N5" t="n">
         <v>0.1</v>
       </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="inlineStr">
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2022-10</t>
         </is>
       </c>
-      <c r="Q5" t="n">
+      <c r="P5" t="n">
         <v>7</v>
       </c>
-      <c r="R5" t="b">
+      <c r="Q5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -837,23 +826,20 @@
         <v>24</v>
       </c>
       <c r="M6" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="N6" t="n">
         <v>0.06</v>
       </c>
-      <c r="O6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" t="inlineStr">
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2022-10</t>
         </is>
       </c>
-      <c r="Q6" t="n">
+      <c r="P6" t="n">
         <v>17</v>
       </c>
-      <c r="R6" t="b">
+      <c r="Q6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -907,23 +893,20 @@
         <v>22</v>
       </c>
       <c r="M7" t="n">
-        <v>3.792</v>
-      </c>
-      <c r="N7" t="n">
         <v>0.31</v>
       </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="inlineStr">
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>2022-08</t>
         </is>
       </c>
-      <c r="Q7" t="n">
+      <c r="P7" t="n">
         <v>14</v>
       </c>
-      <c r="R7" t="b">
+      <c r="Q7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -977,23 +960,20 @@
         <v>30</v>
       </c>
       <c r="M8" t="n">
-        <v>3.505</v>
-      </c>
-      <c r="N8" t="n">
         <v>0.29</v>
       </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="inlineStr">
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr">
         <is>
           <t>2022-07</t>
         </is>
       </c>
-      <c r="Q8" t="n">
+      <c r="P8" t="n">
         <v>10</v>
       </c>
-      <c r="R8" t="b">
+      <c r="Q8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1047,23 +1027,20 @@
         <v>28</v>
       </c>
       <c r="M9" t="n">
-        <v>1.515</v>
-      </c>
-      <c r="N9" t="n">
         <v>0.99</v>
       </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" t="inlineStr">
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>2022-06</t>
         </is>
       </c>
-      <c r="Q9" t="n">
+      <c r="P9" t="n">
         <v>11</v>
       </c>
-      <c r="R9" t="b">
+      <c r="Q9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1117,23 +1094,20 @@
         <v>34</v>
       </c>
       <c r="M10" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>2022-06</t>
         </is>
       </c>
-      <c r="Q10" t="n">
+      <c r="P10" t="n">
         <v>17</v>
       </c>
-      <c r="R10" t="b">
+      <c r="Q10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1186,22 +1160,21 @@
       <c r="L11" t="n">
         <v>34</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>2022-05</t>
         </is>
       </c>
-      <c r="Q11" t="n">
+      <c r="P11" t="n">
         <v>4</v>
       </c>
-      <c r="R11" t="b">
+      <c r="Q11" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1255,19 +1228,18 @@
         <v>26</v>
       </c>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="inlineStr">
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>2022-05</t>
         </is>
       </c>
-      <c r="Q12" t="n">
+      <c r="P12" t="n">
         <v>10</v>
       </c>
-      <c r="R12" t="b">
+      <c r="Q12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1321,19 +1293,18 @@
         <v>22</v>
       </c>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="b">
-        <v>1</v>
-      </c>
-      <c r="P13" t="inlineStr">
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>2022-04</t>
         </is>
       </c>
-      <c r="Q13" t="n">
+      <c r="P13" t="n">
         <v>4</v>
       </c>
-      <c r="R13" t="b">
+      <c r="Q13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1386,22 +1357,19 @@
       <c r="L14" t="n">
         <v>20</v>
       </c>
-      <c r="M14" t="n">
-        <v>2.32</v>
-      </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="b">
-        <v>0</v>
-      </c>
-      <c r="P14" t="inlineStr">
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>2022-04</t>
         </is>
       </c>
-      <c r="Q14" t="n">
+      <c r="P14" t="n">
         <v>16</v>
       </c>
-      <c r="R14" t="b">
+      <c r="Q14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1455,19 +1423,18 @@
         <v>25</v>
       </c>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="b">
-        <v>0</v>
-      </c>
-      <c r="P15" t="inlineStr">
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>2022-04</t>
         </is>
       </c>
-      <c r="Q15" t="n">
+      <c r="P15" t="n">
         <v>4</v>
       </c>
-      <c r="R15" t="b">
+      <c r="Q15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1520,22 +1487,19 @@
       <c r="L16" t="n">
         <v>19</v>
       </c>
-      <c r="M16" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P16" t="inlineStr">
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>2022-04</t>
         </is>
       </c>
-      <c r="Q16" t="n">
+      <c r="P16" t="n">
         <v>15</v>
       </c>
-      <c r="R16" t="b">
+      <c r="Q16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1588,22 +1552,19 @@
       <c r="L17" t="n">
         <v>20</v>
       </c>
-      <c r="M17" t="n">
-        <v>2.09</v>
-      </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="b">
-        <v>0</v>
-      </c>
-      <c r="P17" t="inlineStr">
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr">
         <is>
           <t>2022-04</t>
         </is>
       </c>
-      <c r="Q17" t="n">
+      <c r="P17" t="n">
         <v>5</v>
       </c>
-      <c r="R17" t="b">
+      <c r="Q17" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1657,19 +1618,18 @@
         <v>25</v>
       </c>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="b">
-        <v>1</v>
-      </c>
-      <c r="P18" t="inlineStr">
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" t="inlineStr">
         <is>
           <t>2022-03</t>
         </is>
       </c>
-      <c r="Q18" t="n">
+      <c r="P18" t="n">
         <v>5</v>
       </c>
-      <c r="R18" t="b">
+      <c r="Q18" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1723,23 +1683,20 @@
         <v>15</v>
       </c>
       <c r="M19" t="n">
-        <v>1.009</v>
-      </c>
-      <c r="N19" t="n">
         <v>0.13</v>
       </c>
-      <c r="O19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P19" t="inlineStr">
+      <c r="N19" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>2022-03</t>
         </is>
       </c>
-      <c r="Q19" t="n">
+      <c r="P19" t="n">
         <v>17</v>
       </c>
-      <c r="R19" t="b">
+      <c r="Q19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1793,19 +1750,18 @@
         <v>16</v>
       </c>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="b">
-        <v>0</v>
-      </c>
-      <c r="P20" t="inlineStr">
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" t="inlineStr">
         <is>
           <t>2022-03</t>
         </is>
       </c>
-      <c r="Q20" t="n">
+      <c r="P20" t="n">
         <v>7</v>
       </c>
-      <c r="R20" t="b">
+      <c r="Q20" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1855,23 +1811,20 @@
         <v>19</v>
       </c>
       <c r="M21" t="n">
-        <v>1.321</v>
-      </c>
-      <c r="N21" t="n">
         <v>0.05</v>
       </c>
-      <c r="O21" t="b">
-        <v>0</v>
-      </c>
-      <c r="P21" t="inlineStr">
+      <c r="N21" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q21" t="n">
+      <c r="P21" t="n">
         <v>7</v>
       </c>
-      <c r="R21" t="b">
+      <c r="Q21" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1920,22 +1873,19 @@
       <c r="L22" t="n">
         <v>17</v>
       </c>
-      <c r="M22" t="n">
-        <v>1.271</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="b">
-        <v>0</v>
-      </c>
-      <c r="P22" t="inlineStr">
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q22" t="n">
+      <c r="P22" t="n">
         <v>10</v>
       </c>
-      <c r="R22" t="b">
+      <c r="Q22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1985,23 +1935,20 @@
         <v>9</v>
       </c>
       <c r="M23" t="n">
-        <v>0.498</v>
-      </c>
-      <c r="N23" t="n">
         <v>0.05</v>
       </c>
-      <c r="O23" t="b">
-        <v>0</v>
-      </c>
-      <c r="P23" t="inlineStr">
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q23" t="n">
+      <c r="P23" t="n">
         <v>7</v>
       </c>
-      <c r="R23" t="b">
+      <c r="Q23" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2051,23 +1998,20 @@
         <v>22</v>
       </c>
       <c r="M24" t="n">
-        <v>0.294</v>
-      </c>
-      <c r="N24" t="n">
         <v>0.05</v>
       </c>
-      <c r="O24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P24" t="inlineStr">
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q24" t="n">
+      <c r="P24" t="n">
         <v>11</v>
       </c>
-      <c r="R24" t="b">
+      <c r="Q24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2117,23 +2061,20 @@
         <v>31</v>
       </c>
       <c r="M25" t="n">
-        <v>0.712</v>
-      </c>
-      <c r="N25" t="n">
         <v>0.05</v>
       </c>
-      <c r="O25" t="b">
-        <v>0</v>
-      </c>
-      <c r="P25" t="inlineStr">
+      <c r="N25" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q25" t="n">
+      <c r="P25" t="n">
         <v>18</v>
       </c>
-      <c r="R25" t="b">
+      <c r="Q25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2183,23 +2124,20 @@
         <v>19</v>
       </c>
       <c r="M26" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="N26" t="n">
         <v>0.05</v>
       </c>
-      <c r="O26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P26" t="inlineStr">
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q26" t="n">
+      <c r="P26" t="n">
         <v>9</v>
       </c>
-      <c r="R26" t="b">
+      <c r="Q26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2248,22 +2186,19 @@
       <c r="L27" t="n">
         <v>33</v>
       </c>
-      <c r="M27" t="n">
-        <v>0.711</v>
-      </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="b">
-        <v>0</v>
-      </c>
-      <c r="P27" t="inlineStr">
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr">
         <is>
           <t>2021-11</t>
         </is>
       </c>
-      <c r="Q27" t="n">
+      <c r="P27" t="n">
         <v>3</v>
       </c>
-      <c r="R27" t="b">
+      <c r="Q27" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2311,23 +2246,20 @@
       </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>0.341</v>
-      </c>
-      <c r="N28" t="n">
         <v>0.05</v>
       </c>
-      <c r="O28" t="b">
-        <v>0</v>
-      </c>
-      <c r="P28" t="inlineStr">
+      <c r="N28" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q28" t="n">
+      <c r="P28" t="n">
         <v>5</v>
       </c>
-      <c r="R28" t="b">
+      <c r="Q28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2375,23 +2307,20 @@
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="N29" t="n">
         <v>0.05</v>
       </c>
-      <c r="O29" t="b">
-        <v>0</v>
-      </c>
-      <c r="P29" t="inlineStr">
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q29" t="n">
+      <c r="P29" t="n">
         <v>3</v>
       </c>
-      <c r="R29" t="b">
+      <c r="Q29" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2438,22 +2367,19 @@
         <v>8.4</v>
       </c>
       <c r="L30" t="inlineStr"/>
-      <c r="M30" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="b">
-        <v>0</v>
-      </c>
-      <c r="P30" t="inlineStr">
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="b">
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2500,22 +2426,19 @@
         <v>9.5</v>
       </c>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="b">
-        <v>0</v>
-      </c>
-      <c r="P31" t="inlineStr">
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="b">
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2563,23 +2486,20 @@
       </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="N32" t="n">
         <v>0.05</v>
       </c>
-      <c r="O32" t="b">
-        <v>0</v>
-      </c>
-      <c r="P32" t="inlineStr">
+      <c r="N32" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q32" t="n">
+      <c r="P32" t="n">
         <v>18</v>
       </c>
-      <c r="R32" t="b">
+      <c r="Q32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2627,23 +2547,20 @@
       </c>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="N33" t="n">
         <v>0.05</v>
       </c>
-      <c r="O33" t="b">
-        <v>0</v>
-      </c>
-      <c r="P33" t="inlineStr">
+      <c r="N33" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q33" t="n">
+      <c r="P33" t="n">
         <v>18</v>
       </c>
-      <c r="R33" t="b">
+      <c r="Q33" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2691,23 +2608,20 @@
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="N34" t="n">
         <v>0.05</v>
       </c>
-      <c r="O34" t="b">
-        <v>0</v>
-      </c>
-      <c r="P34" t="inlineStr">
+      <c r="N34" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q34" t="n">
+      <c r="P34" t="n">
         <v>4</v>
       </c>
-      <c r="R34" t="b">
+      <c r="Q34" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2755,23 +2669,20 @@
       </c>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N35" t="n">
         <v>0.05</v>
       </c>
-      <c r="O35" t="b">
-        <v>0</v>
-      </c>
-      <c r="P35" t="inlineStr">
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q35" t="n">
+      <c r="P35" t="n">
         <v>4</v>
       </c>
-      <c r="R35" t="b">
+      <c r="Q35" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2818,22 +2729,19 @@
         <v>8.529999999999999</v>
       </c>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="b">
-        <v>0</v>
-      </c>
-      <c r="P36" t="inlineStr">
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q36" t="n">
+      <c r="P36" t="n">
         <v>5</v>
       </c>
-      <c r="R36" t="b">
+      <c r="Q36" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2880,22 +2788,19 @@
         <v>8.35</v>
       </c>
       <c r="L37" t="inlineStr"/>
-      <c r="M37" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="b">
-        <v>0</v>
-      </c>
-      <c r="P37" t="inlineStr">
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q37" t="n">
+      <c r="P37" t="n">
         <v>5</v>
       </c>
-      <c r="R37" t="b">
+      <c r="Q37" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2942,22 +2847,19 @@
         <v>8.539999999999999</v>
       </c>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="b">
-        <v>0</v>
-      </c>
-      <c r="P38" t="inlineStr">
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q38" t="n">
+      <c r="P38" t="n">
         <v>6</v>
       </c>
-      <c r="R38" t="b">
+      <c r="Q38" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3004,22 +2906,19 @@
         <v>8.609999999999999</v>
       </c>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="b">
-        <v>0</v>
-      </c>
-      <c r="P39" t="inlineStr">
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q39" t="n">
+      <c r="P39" t="n">
         <v>5</v>
       </c>
-      <c r="R39" t="b">
+      <c r="Q39" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3067,23 +2966,20 @@
       </c>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="N40" t="n">
         <v>0.05</v>
       </c>
-      <c r="O40" t="b">
-        <v>0</v>
-      </c>
-      <c r="P40" t="inlineStr">
+      <c r="N40" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q40" t="n">
+      <c r="P40" t="n">
         <v>18</v>
       </c>
-      <c r="R40" t="b">
+      <c r="Q40" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3130,22 +3026,21 @@
         <v>7.59</v>
       </c>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="n">
+      <c r="M41" t="n">
         <v>0.05</v>
       </c>
-      <c r="O41" t="b">
-        <v>0</v>
-      </c>
-      <c r="P41" t="inlineStr">
+      <c r="N41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q41" t="n">
+      <c r="P41" t="n">
         <v>5</v>
       </c>
-      <c r="R41" t="b">
+      <c r="Q41" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3193,23 +3088,20 @@
       </c>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="N42" t="n">
         <v>0.25</v>
       </c>
-      <c r="O42" t="b">
-        <v>0</v>
-      </c>
-      <c r="P42" t="inlineStr">
+      <c r="N42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q42" t="n">
+      <c r="P42" t="n">
         <v>6</v>
       </c>
-      <c r="R42" t="b">
+      <c r="Q42" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3256,22 +3148,19 @@
         <v>8.48</v>
       </c>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="b">
-        <v>0</v>
-      </c>
-      <c r="P43" t="inlineStr">
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q43" t="n">
+      <c r="P43" t="n">
         <v>5</v>
       </c>
-      <c r="R43" t="b">
+      <c r="Q43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3318,22 +3207,19 @@
         <v>8.539999999999999</v>
       </c>
       <c r="L44" t="inlineStr"/>
-      <c r="M44" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="b">
-        <v>0</v>
-      </c>
-      <c r="P44" t="inlineStr">
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q44" t="n">
+      <c r="P44" t="n">
         <v>4</v>
       </c>
-      <c r="R44" t="b">
+      <c r="Q44" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3380,22 +3266,19 @@
         <v>8.109999999999999</v>
       </c>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="n">
-        <v>1.37</v>
-      </c>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="b">
-        <v>0</v>
-      </c>
-      <c r="P45" t="inlineStr">
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q45" t="n">
+      <c r="P45" t="n">
         <v>5</v>
       </c>
-      <c r="R45" t="b">
+      <c r="Q45" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3442,22 +3325,19 @@
         <v>8.51</v>
       </c>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="b">
-        <v>0</v>
-      </c>
-      <c r="P46" t="inlineStr">
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="b">
+        <v>0</v>
+      </c>
+      <c r="O46" t="inlineStr">
         <is>
           <t>2021-09</t>
         </is>
       </c>
-      <c r="Q46" t="n">
+      <c r="P46" t="n">
         <v>5</v>
       </c>
-      <c r="R46" t="b">
+      <c r="Q46" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3503,19 +3383,18 @@
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="b">
-        <v>0</v>
-      </c>
-      <c r="P47" t="inlineStr">
+      <c r="N47" t="b">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q47" t="n">
-        <v>0</v>
-      </c>
-      <c r="R47" t="b">
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3563,19 +3442,18 @@
       </c>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="b">
-        <v>0</v>
-      </c>
-      <c r="P48" t="inlineStr">
+      <c r="N48" t="b">
+        <v>0</v>
+      </c>
+      <c r="O48" t="inlineStr">
         <is>
           <t>2021-06</t>
         </is>
       </c>
-      <c r="Q48" t="n">
-        <v>0</v>
-      </c>
-      <c r="R48" t="b">
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3590,7 +3468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3601,7 +3479,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>serial_num</t>
+          <t>sample_idx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -3656,30 +3534,25 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>tds_ppt</t>
+          <t>ammonia_mg_per_L</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>ammonia_mg_per_L</t>
+          <t>follow_up</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>follow_up</t>
+          <t>month_year</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>month_year</t>
+          <t>hour</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>hour</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>time_mismatch</t>
         </is>
@@ -3728,22 +3601,19 @@
         <v>8.4</v>
       </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="inlineStr">
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3790,22 +3660,19 @@
         <v>9.5</v>
       </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" t="inlineStr">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>2021-10</t>
         </is>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3852,22 +3719,19 @@
         <v>8.44</v>
       </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>1.61</v>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" t="inlineStr">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>2021-08</t>
         </is>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3916,22 +3780,21 @@
       <c r="L5" t="n">
         <v>29</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="inlineStr">
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3981,19 +3844,18 @@
         <v>31</v>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" t="inlineStr">
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4038,22 +3900,21 @@
       <c r="L7" t="n">
         <v>19</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="inlineStr">
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4098,22 +3959,21 @@
       <c r="L8" t="n">
         <v>31</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="inlineStr">
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4162,22 +4022,21 @@
       <c r="L9" t="n">
         <v>29</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" t="inlineStr">
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4226,22 +4085,21 @@
       <c r="L10" t="n">
         <v>26</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" t="inlineStr">
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="b">
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4290,22 +4148,21 @@
       <c r="L11" t="n">
         <v>30</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="b">
-        <v>0</v>
-      </c>
-      <c r="P11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4354,22 +4211,21 @@
       <c r="L12" t="n">
         <v>30</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
+      <c r="M12" t="n">
         <v>0.01</v>
       </c>
-      <c r="O12" t="b">
-        <v>0</v>
-      </c>
-      <c r="P12" t="inlineStr">
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4418,22 +4274,21 @@
       <c r="L13" t="n">
         <v>28</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="b">
-        <v>0</v>
-      </c>
-      <c r="P13" t="inlineStr">
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4479,19 +4334,18 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="b">
-        <v>0</v>
-      </c>
-      <c r="P14" t="inlineStr">
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="b">
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4541,19 +4395,18 @@
         <v>58</v>
       </c>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="b">
-        <v>0</v>
-      </c>
-      <c r="P15" t="inlineStr">
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" t="b">
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4602,22 +4455,21 @@
       <c r="L16" t="n">
         <v>29</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P16" t="inlineStr">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>2021-07</t>
         </is>
       </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="b">
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4665,19 +4517,18 @@
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="b">
-        <v>0</v>
-      </c>
-      <c r="P17" t="inlineStr">
+      <c r="N17" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr">
         <is>
           <t>2021-06</t>
         </is>
       </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4724,22 +4575,21 @@
         <v>8.050000000000001</v>
       </c>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P18" t="inlineStr">
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" t="inlineStr">
         <is>
           <t>2021-06</t>
         </is>
       </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="b">
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>